<commit_message>
feat: Improves formating on the Excel report
also a lot of R# love.
</commit_message>
<xml_diff>
--- a/WhoIsStreaming/Template.xlsx
+++ b/WhoIsStreaming/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WhoIsStreaming\WhoIsStreaming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78923FE-EE28-408D-B53B-7B7424DE91E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A58E88-6381-4D84-B989-A058D4C91332}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{096A6308-3BB2-493F-89F3-4494525C0B3B}"/>
+    <workbookView xWindow="12810" yWindow="4170" windowWidth="21570" windowHeight="13470" xr2:uid="{096A6308-3BB2-493F-89F3-4494525C0B3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>Who Is Streaming?</t>
   </si>
@@ -68,6 +77,9 @@
   </si>
   <si>
     <t>Game Name</t>
+  </si>
+  <si>
+    <t>Viewers x Hours</t>
   </si>
 </sst>
 </file>
@@ -80,7 +92,7 @@
     <numFmt numFmtId="165" formatCode="[h]:mm;@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +131,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -141,7 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -153,6 +173,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -468,7 +489,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32AAA9CB-A8EC-4B1B-A98C-4777CFE7DF14}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -480,24 +501,25 @@
     <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="16.7109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="56.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="56.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -506,7 +528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -515,7 +537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -534,16 +556,19 @@
       <c r="F7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -567,7 +592,8 @@
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="10"/>
+    <col min="7" max="7" width="9.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
@@ -617,7 +643,7 @@
       <c r="F7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="1" t="s">

</xml_diff>

<commit_message>
feat: Excel Report Page with the total viewership by hour.
</commit_message>
<xml_diff>
--- a/WhoIsStreaming/Template.xlsx
+++ b/WhoIsStreaming/Template.xlsx
@@ -1,41 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WhoIsStreaming\WhoIsStreaming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A58E88-6381-4D84-B989-A058D4C91332}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C9C7EE-3E83-48A0-8F8A-22DFBEF403B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12810" yWindow="4170" windowWidth="21570" windowHeight="13470" xr2:uid="{096A6308-3BB2-493F-89F3-4494525C0B3B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{096A6308-3BB2-493F-89F3-4494525C0B3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="1" r:id="rId1"/>
     <sheet name="Observations" sheetId="2" r:id="rId2"/>
+    <sheet name="Viewership" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
     <t>Who Is Streaming?</t>
   </si>
@@ -80,17 +72,24 @@
   </si>
   <si>
     <t>Viewers x Hours</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>Streamers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="[h]:mm;@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm"/>
+    <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ hh"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -161,7 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -174,6 +173,10 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -653,4 +656,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECE0CC2-8D9A-482B-AC57-0ADD28E7E975}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15">
+        <f>MIN($A$9:$A$2006)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="15">
+        <f>MAX($B$8:$B$2005)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix(Report): Fixes an Excel Formula on the new viewership sheet.
</commit_message>
<xml_diff>
--- a/WhoIsStreaming/Template.xlsx
+++ b/WhoIsStreaming/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WhoIsStreaming\WhoIsStreaming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C9C7EE-3E83-48A0-8F8A-22DFBEF403B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A029B8B5-C50C-4827-AE47-58688264D1C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{096A6308-3BB2-493F-89F3-4494525C0B3B}"/>
   </bookViews>
@@ -688,7 +688,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="15">
-        <f>MIN($A$9:$A$2006)</f>
+        <f>MIN($A$8:$A$2006)</f>
         <v>0</v>
       </c>
     </row>
@@ -697,7 +697,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="15">
-        <f>MAX($B$8:$B$2005)</f>
+        <f>MAX($A$8:$A$2005)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>